<commit_message>
Updated UTFSP NSGA II code to accomodate walk matrix
Walk matrix included along with better instance management with json objects
</commit_message>
<xml_diff>
--- a/Input_Data/SSML_Stellenbosch_Data/Dist_matrix/Dist_mx_determination.xlsx
+++ b/Input_Data/SSML_Stellenbosch_Data/Dist_matrix/Dist_mx_determination.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_A0E59EF8EE6D0E1AD7C7A3188A54BDD61B6C8FE5" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DF34133C-D8C3-46D8-AB40-0D0D1760C26D}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="11_A0E59EF8EE6D0E1AD7C7A3188A54BDD61B6C8FE5" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C6E7B93C-7274-4CCE-9BEF-1003694BFAF4}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Driving Dist Matrix" sheetId="1" r:id="rId1"/>
+    <sheet name="Walking Dist Matrix" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>V1</t>
   </si>
@@ -74,6 +75,39 @@
   </si>
   <si>
     <t>TIME: 1200</t>
+  </si>
+  <si>
+    <t>-33.929972, 18.865677</t>
+  </si>
+  <si>
+    <t>-33.930799, 18.85993</t>
+  </si>
+  <si>
+    <t>-33.935169, 18.86132</t>
+  </si>
+  <si>
+    <t>-33.936725, 18.866079</t>
+  </si>
+  <si>
+    <t>-33.934916, 18.871437</t>
+  </si>
+  <si>
+    <t>-33.933425, 18.870353</t>
+  </si>
+  <si>
+    <t>-33.930843, 18.871007</t>
+  </si>
+  <si>
+    <t>-33.932234, 18.86467</t>
+  </si>
+  <si>
+    <t>-33.934052, 18.865602</t>
+  </si>
+  <si>
+    <t>-33.940034, 18.870718</t>
+  </si>
+  <si>
+    <t>DRIVING DIST MATRIX FOR COMPARISON</t>
   </si>
 </sst>
 </file>
@@ -416,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13:Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1761,10 +1795,1391 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD415E3-5E43-42DF-BD42-6D050D44CDD8}">
+  <dimension ref="A1:Q37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13:Q23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.140625" customWidth="1"/>
+    <col min="9" max="9" width="4" customWidth="1"/>
+    <col min="10" max="17" width="4.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="2">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1">
+        <v>4</v>
+      </c>
+      <c r="M1" s="1">
+        <v>5</v>
+      </c>
+      <c r="N1" s="1">
+        <v>6</v>
+      </c>
+      <c r="O1" s="2">
+        <v>7</v>
+      </c>
+      <c r="P1" s="2">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>-33.929971999999999</v>
+      </c>
+      <c r="D2">
+        <v>18.865677000000002</v>
+      </c>
+      <c r="E2" t="str">
+        <f>CONCATENATE(C2,", ",D2)</f>
+        <v>-33.929972, 18.865677</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>-33.930799</v>
+      </c>
+      <c r="D3">
+        <v>18.859929999999999</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E10" si="0">CONCATENATE(C3,", ",D3)</f>
+        <v>-33.930799, 18.85993</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>-33.935169000000002</v>
+      </c>
+      <c r="D4">
+        <v>18.861319999999999</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>-33.935169, 18.86132</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>-33.936725000000003</v>
+      </c>
+      <c r="D5">
+        <v>18.866078999999999</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>-33.936725, 18.866079</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>-33.934916000000001</v>
+      </c>
+      <c r="D6">
+        <v>18.871437</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>-33.934916, 18.871437</v>
+      </c>
+      <c r="G6" s="1">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>1</v>
+      </c>
+      <c r="P6" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>-33.933425</v>
+      </c>
+      <c r="D7">
+        <v>18.870353000000001</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>-33.933425, 18.870353</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>1</v>
+      </c>
+      <c r="P7" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>-33.930843000000003</v>
+      </c>
+      <c r="D8">
+        <v>18.871006999999999</v>
+      </c>
+      <c r="E8" t="str">
+        <f>CONCATENATE(C8,", ",D8)</f>
+        <v>-33.930843, 18.871007</v>
+      </c>
+      <c r="G8" s="1">
+        <v>6</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <v>1</v>
+      </c>
+      <c r="P8" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>-33.932234000000001</v>
+      </c>
+      <c r="D9">
+        <v>18.86467</v>
+      </c>
+      <c r="E9" t="str">
+        <f>CONCATENATE(C9,", ",D9)</f>
+        <v>-33.932234, 18.86467</v>
+      </c>
+      <c r="G9" s="2">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1</v>
+      </c>
+      <c r="N9" s="1">
+        <v>1</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>-33.934052000000001</v>
+      </c>
+      <c r="D10">
+        <v>18.865601999999999</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>-33.934052, 18.865602</v>
+      </c>
+      <c r="G10" s="2">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1</v>
+      </c>
+      <c r="N10" s="1">
+        <v>1</v>
+      </c>
+      <c r="O10" s="1">
+        <v>1</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>-33.940033999999997</v>
+      </c>
+      <c r="D11">
+        <v>18.870718</v>
+      </c>
+      <c r="E11" t="str">
+        <f>CONCATENATE(C11,", ",D11)</f>
+        <v>-33.940034, 18.870718</v>
+      </c>
+      <c r="G11" s="2">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1</v>
+      </c>
+      <c r="P11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G13" s="1"/>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2">
+        <v>2</v>
+      </c>
+      <c r="K13" s="1">
+        <v>3</v>
+      </c>
+      <c r="L13" s="1">
+        <v>4</v>
+      </c>
+      <c r="M13" s="1">
+        <v>5</v>
+      </c>
+      <c r="N13" s="1">
+        <v>6</v>
+      </c>
+      <c r="O13" s="2">
+        <v>7</v>
+      </c>
+      <c r="P13" s="2">
+        <v>8</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>6</v>
+      </c>
+      <c r="J14" s="1">
+        <v>12</v>
+      </c>
+      <c r="K14" s="1">
+        <v>12</v>
+      </c>
+      <c r="L14" s="1">
+        <v>14</v>
+      </c>
+      <c r="M14" s="1">
+        <v>10</v>
+      </c>
+      <c r="N14" s="1">
+        <v>10</v>
+      </c>
+      <c r="O14" s="1">
+        <v>4</v>
+      </c>
+      <c r="P14" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1">
+        <v>6</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>7</v>
+      </c>
+      <c r="K15" s="1">
+        <v>15</v>
+      </c>
+      <c r="L15" s="1">
+        <v>20</v>
+      </c>
+      <c r="M15" s="1">
+        <v>17</v>
+      </c>
+      <c r="N15" s="1">
+        <v>15</v>
+      </c>
+      <c r="O15" s="1">
+        <v>8</v>
+      </c>
+      <c r="P15" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="2">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1">
+        <v>12</v>
+      </c>
+      <c r="I16" s="1">
+        <v>7</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>8</v>
+      </c>
+      <c r="L16" s="1">
+        <v>15</v>
+      </c>
+      <c r="M16" s="1">
+        <v>12</v>
+      </c>
+      <c r="N16" s="1">
+        <v>16</v>
+      </c>
+      <c r="O16" s="1">
+        <v>8</v>
+      </c>
+      <c r="P16" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3</v>
+      </c>
+      <c r="H17" s="1">
+        <v>12</v>
+      </c>
+      <c r="I17" s="1">
+        <v>15</v>
+      </c>
+      <c r="J17" s="1">
+        <v>8</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>8</v>
+      </c>
+      <c r="M17" s="1">
+        <v>10</v>
+      </c>
+      <c r="N17" s="1">
+        <v>14</v>
+      </c>
+      <c r="O17" s="1">
+        <v>8</v>
+      </c>
+      <c r="P17" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="1">
+        <v>4</v>
+      </c>
+      <c r="H18" s="1">
+        <v>14</v>
+      </c>
+      <c r="I18" s="1">
+        <v>20</v>
+      </c>
+      <c r="J18" s="1">
+        <v>15</v>
+      </c>
+      <c r="K18" s="1">
+        <v>8</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>3</v>
+      </c>
+      <c r="N18" s="1">
+        <v>11</v>
+      </c>
+      <c r="O18" s="1">
+        <v>11</v>
+      </c>
+      <c r="P18" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="1">
+        <v>5</v>
+      </c>
+      <c r="H19" s="1">
+        <v>10</v>
+      </c>
+      <c r="I19" s="1">
+        <v>17</v>
+      </c>
+      <c r="J19" s="1">
+        <v>12</v>
+      </c>
+      <c r="K19" s="1">
+        <v>10</v>
+      </c>
+      <c r="L19" s="1">
+        <v>3</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <v>9</v>
+      </c>
+      <c r="O19" s="1">
+        <v>8</v>
+      </c>
+      <c r="P19" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="1">
+        <v>6</v>
+      </c>
+      <c r="H20" s="1">
+        <v>10</v>
+      </c>
+      <c r="I20" s="1">
+        <v>15</v>
+      </c>
+      <c r="J20" s="1">
+        <v>16</v>
+      </c>
+      <c r="K20" s="1">
+        <v>14</v>
+      </c>
+      <c r="L20" s="1">
+        <v>11</v>
+      </c>
+      <c r="M20" s="1">
+        <v>9</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
+        <v>8</v>
+      </c>
+      <c r="P20" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="2">
+        <v>7</v>
+      </c>
+      <c r="H21" s="1">
+        <v>4</v>
+      </c>
+      <c r="I21" s="1">
+        <v>8</v>
+      </c>
+      <c r="J21" s="1">
+        <v>8</v>
+      </c>
+      <c r="K21" s="1">
+        <v>8</v>
+      </c>
+      <c r="L21" s="1">
+        <v>11</v>
+      </c>
+      <c r="M21" s="1">
+        <v>8</v>
+      </c>
+      <c r="N21" s="1">
+        <v>8</v>
+      </c>
+      <c r="O21" s="1">
+        <v>0</v>
+      </c>
+      <c r="P21" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="2">
+        <v>8</v>
+      </c>
+      <c r="H22" s="1">
+        <v>8</v>
+      </c>
+      <c r="I22" s="1">
+        <v>11</v>
+      </c>
+      <c r="J22" s="1">
+        <v>7</v>
+      </c>
+      <c r="K22" s="1">
+        <v>4</v>
+      </c>
+      <c r="L22" s="1">
+        <v>8</v>
+      </c>
+      <c r="M22" s="1">
+        <v>5</v>
+      </c>
+      <c r="N22" s="1">
+        <v>10</v>
+      </c>
+      <c r="O22" s="1">
+        <v>4</v>
+      </c>
+      <c r="P22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="2">
+        <v>9</v>
+      </c>
+      <c r="H23" s="1">
+        <v>19</v>
+      </c>
+      <c r="I23" s="1">
+        <v>24</v>
+      </c>
+      <c r="J23" s="1">
+        <v>17</v>
+      </c>
+      <c r="K23" s="1">
+        <v>9</v>
+      </c>
+      <c r="L23" s="1">
+        <v>9</v>
+      </c>
+      <c r="M23" s="1">
+        <v>12</v>
+      </c>
+      <c r="N23" s="1">
+        <v>18</v>
+      </c>
+      <c r="O23" s="1">
+        <v>17</v>
+      </c>
+      <c r="P23" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="G27" s="1"/>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="J27" s="2">
+        <v>2</v>
+      </c>
+      <c r="K27" s="1">
+        <v>3</v>
+      </c>
+      <c r="L27" s="1">
+        <v>4</v>
+      </c>
+      <c r="M27" s="1">
+        <v>5</v>
+      </c>
+      <c r="N27" s="1">
+        <v>6</v>
+      </c>
+      <c r="O27" s="2">
+        <v>7</v>
+      </c>
+      <c r="P27" s="2">
+        <v>8</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1">
+        <v>2</v>
+      </c>
+      <c r="J28" s="1">
+        <v>4</v>
+      </c>
+      <c r="K28" s="1">
+        <v>3</v>
+      </c>
+      <c r="L28" s="1">
+        <v>4</v>
+      </c>
+      <c r="M28" s="1">
+        <v>3</v>
+      </c>
+      <c r="N28" s="1">
+        <v>2</v>
+      </c>
+      <c r="O28" s="1">
+        <v>2</v>
+      </c>
+      <c r="P28" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1">
+        <v>2</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
+      <c r="J29" s="1">
+        <v>3</v>
+      </c>
+      <c r="K29" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L29" s="1">
+        <v>10000</v>
+      </c>
+      <c r="M29" s="1">
+        <v>10000</v>
+      </c>
+      <c r="N29" s="1">
+        <v>10000</v>
+      </c>
+      <c r="O29" s="1">
+        <v>3</v>
+      </c>
+      <c r="P29" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="G30" s="2">
+        <v>2</v>
+      </c>
+      <c r="H30" s="1">
+        <v>4</v>
+      </c>
+      <c r="I30" s="1">
+        <v>3</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1">
+        <v>3</v>
+      </c>
+      <c r="L30" s="1">
+        <v>4</v>
+      </c>
+      <c r="M30" s="1">
+        <v>3</v>
+      </c>
+      <c r="N30" s="1">
+        <v>4</v>
+      </c>
+      <c r="O30" s="1">
+        <v>3</v>
+      </c>
+      <c r="P30" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="G31" s="1">
+        <v>3</v>
+      </c>
+      <c r="H31" s="1">
+        <v>3</v>
+      </c>
+      <c r="I31" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J31" s="1">
+        <v>3</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0</v>
+      </c>
+      <c r="L31" s="1">
+        <v>10000</v>
+      </c>
+      <c r="M31" s="1">
+        <v>10000</v>
+      </c>
+      <c r="N31" s="1">
+        <v>10000</v>
+      </c>
+      <c r="O31" s="1">
+        <v>3</v>
+      </c>
+      <c r="P31" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="G32" s="1">
+        <v>4</v>
+      </c>
+      <c r="H32" s="1">
+        <v>4</v>
+      </c>
+      <c r="I32" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J32" s="1">
+        <v>4</v>
+      </c>
+      <c r="K32" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L32" s="1">
+        <v>0</v>
+      </c>
+      <c r="M32" s="1">
+        <v>10000</v>
+      </c>
+      <c r="N32" s="1">
+        <v>10000</v>
+      </c>
+      <c r="O32" s="1">
+        <v>4</v>
+      </c>
+      <c r="P32" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G33" s="1">
+        <v>5</v>
+      </c>
+      <c r="H33" s="1">
+        <v>3</v>
+      </c>
+      <c r="I33" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J33" s="1">
+        <v>3</v>
+      </c>
+      <c r="K33" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L33" s="1">
+        <v>10000</v>
+      </c>
+      <c r="M33" s="1">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1">
+        <v>10000</v>
+      </c>
+      <c r="O33" s="1">
+        <v>3</v>
+      </c>
+      <c r="P33" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G34" s="1">
+        <v>6</v>
+      </c>
+      <c r="H34" s="1">
+        <v>2</v>
+      </c>
+      <c r="I34" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J34" s="1">
+        <v>4</v>
+      </c>
+      <c r="K34" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L34" s="1">
+        <v>10000</v>
+      </c>
+      <c r="M34" s="1">
+        <v>10000</v>
+      </c>
+      <c r="N34" s="1">
+        <v>0</v>
+      </c>
+      <c r="O34" s="1">
+        <v>2</v>
+      </c>
+      <c r="P34" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G35" s="2">
+        <v>7</v>
+      </c>
+      <c r="H35" s="1">
+        <v>2</v>
+      </c>
+      <c r="I35" s="1">
+        <v>3</v>
+      </c>
+      <c r="J35" s="1">
+        <v>3</v>
+      </c>
+      <c r="K35" s="1">
+        <v>3</v>
+      </c>
+      <c r="L35" s="1">
+        <v>4</v>
+      </c>
+      <c r="M35" s="1">
+        <v>3</v>
+      </c>
+      <c r="N35" s="1">
+        <v>2</v>
+      </c>
+      <c r="O35" s="1">
+        <v>0</v>
+      </c>
+      <c r="P35" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G36" s="2">
+        <v>8</v>
+      </c>
+      <c r="H36" s="1">
+        <v>3</v>
+      </c>
+      <c r="I36" s="1">
+        <v>4</v>
+      </c>
+      <c r="J36" s="1">
+        <v>2</v>
+      </c>
+      <c r="K36" s="1">
+        <v>1</v>
+      </c>
+      <c r="L36" s="1">
+        <v>3</v>
+      </c>
+      <c r="M36" s="1">
+        <v>2</v>
+      </c>
+      <c r="N36" s="1">
+        <v>2</v>
+      </c>
+      <c r="O36" s="1">
+        <v>3</v>
+      </c>
+      <c r="P36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G37" s="2">
+        <v>9</v>
+      </c>
+      <c r="H37" s="1">
+        <v>5</v>
+      </c>
+      <c r="I37" s="1">
+        <v>6</v>
+      </c>
+      <c r="J37" s="1">
+        <v>5</v>
+      </c>
+      <c r="K37" s="1">
+        <v>3</v>
+      </c>
+      <c r="L37" s="1">
+        <v>4</v>
+      </c>
+      <c r="M37" s="1">
+        <v>4</v>
+      </c>
+      <c r="N37" s="1">
+        <v>4</v>
+      </c>
+      <c r="O37" s="1">
+        <v>5</v>
+      </c>
+      <c r="P37" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1991,27 +3406,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECABE974-D70C-4B85-91EA-3F27AFA95AD9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA37B58E-DB46-4F54-8727-1F94C311485C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="72c0c944-1be0-4f2a-9ab5-054190dce639"/>
-    <ds:schemaRef ds:uri="ef5f2f6b-70ed-4864-9ace-de76c50c9c1f"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2036,9 +3439,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA37B58E-DB46-4F54-8727-1F94C311485C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECABE974-D70C-4B85-91EA-3F27AFA95AD9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="72c0c944-1be0-4f2a-9ab5-054190dce639"/>
+    <ds:schemaRef ds:uri="ef5f2f6b-70ed-4864-9ace-de76c50c9c1f"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>